<commit_message>
FIX: Issues with trigonometric functions
* Right branch for ACOT for negative numbers
* correct error for ACOTH
* Correct approx for COTH for x > 20
</commit_message>
<xml_diff>
--- a/xlsx/tests/calc_tests/trigonometric_functions.xlsx
+++ b/xlsx/tests/calc_tests/trigonometric_functions.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7402B554-18A9-4DE4-B480-E1568F7AE3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48796FBC-6187-4010-BE1A-E3B595E83285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31280" windowHeight="12950" xr2:uid="{8EEA0296-F25F-4633-ADCF-E78FA5A505D5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31280" windowHeight="12950" firstSheet="1" xr2:uid="{8EEA0296-F25F-4633-ADCF-E78FA5A505D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LargeValues" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>SIN</t>
   </si>
@@ -74,13 +75,31 @@
     <t>ATANH</t>
   </si>
   <si>
+    <t>ACOT</t>
+  </si>
+  <si>
+    <t>ACOTH</t>
+  </si>
+  <si>
+    <t>CSC</t>
+  </si>
+  <si>
+    <t>CSCH</t>
+  </si>
+  <si>
+    <t>SECH</t>
+  </si>
+  <si>
     <t>qwerty</t>
+  </si>
+  <si>
+    <t>=CSC(A12)</t>
   </si>
   <si>
     <t>=TAN(A13)</t>
   </si>
   <si>
-    <t>NOTE: Excel fails slightly with the TAN(PI/2) (ie does not follow IEEE 754)</t>
+    <t>COTH</t>
   </si>
 </sst>
 </file>
@@ -153,11 +172,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -178,7 +196,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -466,7 +484,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -474,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216F1871-D94A-4C42-940B-9397DB6A9E02}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -492,7 +510,7 @@
     <col min="11" max="11" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15">
+    <row r="1" spans="1:18" ht="15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -530,8 +548,23 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15">
       <c r="A2">
         <v>5</v>
       </c>
@@ -583,8 +616,28 @@
         <f>ATANH(A2)</f>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15">
+      <c r="N2" s="2">
+        <f>_xlfn.ACOT(A2)</f>
+        <v>0.19739555984988078</v>
+      </c>
+      <c r="O2" s="2">
+        <f>_xlfn.ACOTH(A2)</f>
+        <v>0.20273255405408222</v>
+      </c>
+      <c r="P2" s="2">
+        <f>_xlfn.CSC(A2)</f>
+        <v>-1.0428352127714058</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>_xlfn.CSCH(A2)</f>
+        <v>1.3476505830589089E-2</v>
+      </c>
+      <c r="R2" s="2">
+        <f>_xlfn.SECH(A2)</f>
+        <v>1.3475282221304556E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15">
       <c r="A3">
         <v>2.8</v>
       </c>
@@ -636,8 +689,28 @@
         <f t="shared" ref="M3:M15" si="11">ATANH(A3)</f>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15">
+      <c r="N3" s="2">
+        <f t="shared" ref="N3:N18" si="12">_xlfn.ACOT(A3)</f>
+        <v>0.34302394042070339</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:O18" si="13">_xlfn.ACOTH(A3)</f>
+        <v>0.37360720091511057</v>
+      </c>
+      <c r="P3" s="2">
+        <f t="shared" ref="P3:P18" si="14">_xlfn.CSC(A3)</f>
+        <v>2.9851802206573432</v>
+      </c>
+      <c r="Q3" s="2">
+        <f t="shared" ref="Q3:Q18" si="15">_xlfn.CSCH(A3)</f>
+        <v>0.122071529128817</v>
+      </c>
+      <c r="R3" s="2">
+        <f t="shared" ref="R3:R18" si="16">_xlfn.SECH(A3)</f>
+        <v>0.12117204753241388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15">
       <c r="A4">
         <v>-3</v>
       </c>
@@ -689,8 +762,28 @@
         <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="15">
+      <c r="N4" s="2">
+        <f t="shared" si="12"/>
+        <v>2.819842099193151</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" si="13"/>
+        <v>-0.34657359027997264</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" si="14"/>
+        <v>-7.0861673957371867</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" si="15"/>
+        <v>-9.9821569668822732E-2</v>
+      </c>
+      <c r="R4" s="2">
+        <f t="shared" si="16"/>
+        <v>9.9327927419433207E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15">
       <c r="A5">
         <v>0.123</v>
       </c>
@@ -742,8 +835,28 @@
         <f t="shared" si="11"/>
         <v>0.12362598118313008</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="15">
+      <c r="N5" s="2">
+        <f t="shared" si="12"/>
+        <v>1.4484110453230941</v>
+      </c>
+      <c r="O5" s="2" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="14"/>
+        <v>8.1506175421487992</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" si="15"/>
+        <v>8.1096174267060963</v>
+      </c>
+      <c r="R5" s="2">
+        <f t="shared" si="16"/>
+        <v>0.99248289312717008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15">
       <c r="A6">
         <v>-0.5</v>
       </c>
@@ -795,8 +908,28 @@
         <f t="shared" si="11"/>
         <v>-0.54930614433405489</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="15">
+      <c r="N6" s="2">
+        <f t="shared" si="12"/>
+        <v>2.0344439357957027</v>
+      </c>
+      <c r="O6" s="2" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="14"/>
+        <v>-2.0858296429334882</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="15"/>
+        <v>-1.9190347513349437</v>
+      </c>
+      <c r="R6" s="2">
+        <f t="shared" si="16"/>
+        <v>0.88681888397007402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15">
       <c r="A7" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
@@ -849,8 +982,28 @@
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="15">
+      <c r="N7" s="2" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O7" s="2" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="2" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q7" s="2" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R7" s="2" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15">
       <c r="A8">
         <v>100</v>
       </c>
@@ -902,8 +1055,28 @@
         <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="15">
+      <c r="N8" s="2">
+        <f t="shared" si="12"/>
+        <v>9.9996666866652376E-3</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="13"/>
+        <v>1.0000333353334763E-2</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="14"/>
+        <v>-1.9748575314240999</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="15"/>
+        <v>7.4401519520416712E-44</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="16"/>
+        <v>7.4401519520416712E-44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -955,10 +1128,30 @@
         <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="15">
+      <c r="N9" s="2">
+        <f t="shared" si="12"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="O9" s="2" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="14"/>
+        <v>1.1883951057781212</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="15"/>
+        <v>0.85091812823932156</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="16"/>
+        <v>0.64805427366388546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="e">
         <f t="shared" si="0"/>
@@ -1008,8 +1201,28 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="15">
+      <c r="N10" s="2" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O10" s="2" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P10" s="2" t="e">
+        <f t="shared" si="14"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q10" s="2" t="e">
+        <f t="shared" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R10" s="2" t="e">
+        <f t="shared" si="16"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1061,8 +1274,28 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="15">
+      <c r="N11" s="2">
+        <f t="shared" si="12"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="O11" s="2" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P11" s="2" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q11" s="2" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15">
       <c r="A12" s="2">
         <f>PI()</f>
         <v>3.1415926535897931</v>
@@ -1115,8 +1348,27 @@
         <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="15">
+      <c r="N12" s="2">
+        <f t="shared" si="12"/>
+        <v>0.30816907111598496</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="13"/>
+        <v>0.32976531495669914</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="15"/>
+        <v>8.6589537530046945E-2</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="16"/>
+        <v>8.6266738334054432E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15">
       <c r="A13" s="2">
         <f>PI()/2</f>
         <v>1.5707963267948966</v>
@@ -1129,8 +1381,8 @@
         <f t="shared" si="1"/>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>13</v>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E13" s="2" t="e">
         <f t="shared" si="3"/>
@@ -1168,8 +1420,28 @@
         <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="15">
+      <c r="N13" s="2">
+        <f t="shared" si="12"/>
+        <v>0.56691150494100939</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="13"/>
+        <v>0.75246926714192719</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="15"/>
+        <v>0.43453720809469581</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="16"/>
+        <v>0.3985368153383867</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15">
       <c r="A14" s="2">
         <f>PI()/4</f>
         <v>0.78539816339744828</v>
@@ -1222,8 +1494,28 @@
         <f t="shared" si="11"/>
         <v>1.059306170823243</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="15">
+      <c r="N14" s="2">
+        <f t="shared" si="12"/>
+        <v>0.90502257676654274</v>
+      </c>
+      <c r="O14" s="2" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="14"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="15"/>
+        <v>1.1511838709208486</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="16"/>
+        <v>0.7549397087141313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15">
       <c r="A15">
         <v>61</v>
       </c>
@@ -1275,8 +1567,28 @@
         <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="15">
+      <c r="N15" s="2">
+        <f t="shared" si="12"/>
+        <v>1.6391974308005267E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="13"/>
+        <v>1.6394911411495437E-2</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="14"/>
+        <v>-1.0350704966241462</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="15"/>
+        <v>6.4426805719850326E-27</v>
+      </c>
+      <c r="R15" s="2">
+        <f t="shared" si="16"/>
+        <v>6.4426805719850326E-27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1285,51 +1597,71 @@
         <v>0.8414709848078965</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" ref="C16" si="12">COS(A16)</f>
+        <f t="shared" ref="C16" si="17">COS(A16)</f>
         <v>0.54030230586813977</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" ref="D16" si="13">TAN(A16)</f>
+        <f t="shared" ref="D16" si="18">TAN(A16)</f>
         <v>1.5574077246549023</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" ref="E16" si="14">ASIN(A16)</f>
+        <f t="shared" ref="E16" si="19">ASIN(A16)</f>
         <v>1.5707963267948966</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" ref="F16" si="15">ACOS(A16)</f>
+        <f t="shared" ref="F16" si="20">ACOS(A16)</f>
         <v>0</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" ref="G16" si="16">ATAN(A16)</f>
+        <f t="shared" ref="G16" si="21">ATAN(A16)</f>
         <v>0.78539816339744828</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" ref="H16" si="17">SINH(A16)</f>
+        <f t="shared" ref="H16" si="22">SINH(A16)</f>
         <v>1.1752011936438014</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" ref="I16" si="18">COSH(A16)</f>
+        <f t="shared" ref="I16" si="23">COSH(A16)</f>
         <v>1.5430806348152437</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" ref="J16" si="19">TANH(A16)</f>
+        <f t="shared" ref="J16" si="24">TANH(A16)</f>
         <v>0.76159415595576485</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" ref="K16" si="20">ASINH(A16)</f>
+        <f t="shared" ref="K16" si="25">ASINH(A16)</f>
         <v>0.88137358701954294</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" ref="L16" si="21">ACOSH(A16)</f>
+        <f t="shared" ref="L16" si="26">ACOSH(A16)</f>
         <v>0</v>
       </c>
       <c r="M16" s="2" t="e">
-        <f t="shared" ref="M16" si="22">ATANH(A16)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15">
+        <f t="shared" ref="M16" si="27">ATANH(A16)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="12"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="O16" s="2" t="e">
+        <f t="shared" si="13"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="14"/>
+        <v>1.1883951057781212</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="15"/>
+        <v>0.85091812823932156</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" si="16"/>
+        <v>0.64805427366388546</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15">
       <c r="A17" t="e">
         <f>NA()</f>
         <v>#N/A</v>
@@ -1339,51 +1671,71 @@
         <v>#N/A</v>
       </c>
       <c r="C17" s="2" t="e">
-        <f t="shared" ref="C17" si="23">COS(A17)</f>
+        <f t="shared" ref="C17" si="28">COS(A17)</f>
         <v>#N/A</v>
       </c>
       <c r="D17" s="2" t="e">
-        <f t="shared" ref="D17" si="24">TAN(A17)</f>
+        <f t="shared" ref="D17" si="29">TAN(A17)</f>
         <v>#N/A</v>
       </c>
       <c r="E17" s="2" t="e">
-        <f t="shared" ref="E17" si="25">ASIN(A17)</f>
+        <f t="shared" ref="E17" si="30">ASIN(A17)</f>
         <v>#N/A</v>
       </c>
       <c r="F17" s="2" t="e">
-        <f t="shared" ref="F17" si="26">ACOS(A17)</f>
+        <f t="shared" ref="F17" si="31">ACOS(A17)</f>
         <v>#N/A</v>
       </c>
       <c r="G17" s="2" t="e">
-        <f t="shared" ref="G17" si="27">ATAN(A17)</f>
+        <f t="shared" ref="G17" si="32">ATAN(A17)</f>
         <v>#N/A</v>
       </c>
       <c r="H17" s="2" t="e">
-        <f t="shared" ref="H17" si="28">SINH(A17)</f>
+        <f t="shared" ref="H17" si="33">SINH(A17)</f>
         <v>#N/A</v>
       </c>
       <c r="I17" s="2" t="e">
-        <f t="shared" ref="I17" si="29">COSH(A17)</f>
+        <f t="shared" ref="I17" si="34">COSH(A17)</f>
         <v>#N/A</v>
       </c>
       <c r="J17" s="2" t="e">
-        <f t="shared" ref="J17" si="30">TANH(A17)</f>
+        <f t="shared" ref="J17" si="35">TANH(A17)</f>
         <v>#N/A</v>
       </c>
       <c r="K17" s="2" t="e">
-        <f t="shared" ref="K17" si="31">ASINH(A17)</f>
+        <f t="shared" ref="K17" si="36">ASINH(A17)</f>
         <v>#N/A</v>
       </c>
       <c r="L17" s="2" t="e">
-        <f t="shared" ref="L17" si="32">ACOSH(A17)</f>
+        <f t="shared" ref="L17" si="37">ACOSH(A17)</f>
         <v>#N/A</v>
       </c>
       <c r="M17" s="2" t="e">
-        <f t="shared" ref="M17" si="33">ATANH(A17)</f>
+        <f t="shared" ref="M17" si="38">ATANH(A17)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15">
+      <c r="N17" s="2" t="e">
+        <f t="shared" si="12"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O17" s="2" t="e">
+        <f t="shared" si="13"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P17" s="2" t="e">
+        <f t="shared" si="14"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q17" s="2" t="e">
+        <f t="shared" si="15"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R17" s="2" t="e">
+        <f t="shared" si="16"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15">
       <c r="A18">
         <v>-7.1230000000000002</v>
       </c>
@@ -1392,95 +1744,727 @@
         <v>-0.74451942153277462</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18" si="34">COS(A18)</f>
+        <f t="shared" ref="C18" si="39">COS(A18)</f>
         <v>0.66760080209695871</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" ref="D18" si="35">TAN(A18)</f>
+        <f t="shared" ref="D18" si="40">TAN(A18)</f>
         <v>-1.115216487449104</v>
       </c>
       <c r="E18" s="2" t="e">
-        <f t="shared" ref="E18" si="36">ASIN(A18)</f>
+        <f t="shared" ref="E18" si="41">ASIN(A18)</f>
         <v>#NUM!</v>
       </c>
       <c r="F18" s="2" t="e">
-        <f t="shared" ref="F18" si="37">ACOS(A18)</f>
+        <f t="shared" ref="F18" si="42">ACOS(A18)</f>
         <v>#NUM!</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" ref="G18" si="38">ATAN(A18)</f>
+        <f t="shared" ref="G18" si="43">ATAN(A18)</f>
         <v>-1.4313176233874174</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" ref="H18" si="39">SINH(A18)</f>
+        <f t="shared" ref="H18" si="44">SINH(A18)</f>
         <v>-620.08227400854867</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" ref="I18" si="40">COSH(A18)</f>
+        <f t="shared" ref="I18" si="45">COSH(A18)</f>
         <v>620.08308035263531</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" ref="J18" si="41">TANH(A18)</f>
+        <f t="shared" ref="J18" si="46">TANH(A18)</f>
         <v>-0.99999869961927335</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" ref="K18" si="42">ASINH(A18)</f>
+        <f t="shared" ref="K18" si="47">ASINH(A18)</f>
         <v>-2.6613674989835281</v>
       </c>
       <c r="L18" s="2" t="e">
-        <f t="shared" ref="L18" si="43">ACOSH(A18)</f>
+        <f t="shared" ref="L18" si="48">ACOSH(A18)</f>
         <v>#NUM!</v>
       </c>
       <c r="M18" s="2" t="e">
-        <f t="shared" ref="M18" si="44">ATANH(A18)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+        <f t="shared" ref="M18" si="49">ATANH(A18)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="12"/>
+        <v>3.0021139501823138</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="13"/>
+        <v>-0.14132368578649973</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="14"/>
+        <v>-1.3431483062473459</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="15"/>
+        <v>-1.6126892219244663E-3</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="16"/>
+        <v>1.6126871248144839E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" ref="B19" si="50">SIN(A19)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" ref="C19" si="51">COS(A19)</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" ref="D19" si="52">TAN(A19)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" ref="E19" si="53">ASIN(A19)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" ref="F19" si="54">ACOS(A19)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" ref="G19" si="55">ATAN(A19)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" ref="H19" si="56">SINH(A19)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" ref="I19" si="57">COSH(A19)</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" ref="J19" si="58">TANH(A19)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" ref="K19" si="59">ASINH(A19)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="e">
+        <f t="shared" ref="L19" si="60">ACOSH(A19)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" ref="M19" si="61">ATANH(A19)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" ref="N19" si="62">_xlfn.ACOT(A19)</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="O19" s="2" t="e">
+        <f t="shared" ref="O19" si="63">_xlfn.ACOTH(A19)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P19" s="2" t="e">
+        <f t="shared" ref="P19" si="64">_xlfn.CSC(A19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q19" s="2" t="e">
+        <f t="shared" ref="Q19" si="65">_xlfn.CSCH(A19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R19" s="2">
+        <f t="shared" ref="R19" si="66">_xlfn.SECH(A19)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" ref="B20:B26" si="67">SIN(A20)</f>
+        <v>0.90929742682568171</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" ref="C20:C26" si="68">COS(A20)</f>
+        <v>-0.41614683654714241</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" ref="D20:D26" si="69">TAN(A20)</f>
+        <v>-2.1850398632615189</v>
+      </c>
+      <c r="E20" s="2" t="e">
+        <f t="shared" ref="E20:E26" si="70">ASIN(A20)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F20" s="2" t="e">
+        <f t="shared" ref="F20:F26" si="71">ACOS(A20)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" ref="G20:G26" si="72">ATAN(A20)</f>
+        <v>1.1071487177940904</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" ref="H20:H26" si="73">SINH(A20)</f>
+        <v>3.626860407847019</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" ref="I20:I26" si="74">COSH(A20)</f>
+        <v>3.7621956910836314</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" ref="J20:J26" si="75">TANH(A20)</f>
+        <v>0.96402758007581701</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" ref="K20:K26" si="76">ASINH(A20)</f>
+        <v>1.4436354751788103</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" ref="L20:L26" si="77">ACOSH(A20)</f>
+        <v>1.3169578969248166</v>
+      </c>
+      <c r="M20" s="2" t="e">
+        <f t="shared" ref="M20:M26" si="78">ATANH(A20)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" ref="N20:N26" si="79">_xlfn.ACOT(A20)</f>
+        <v>0.46364760900080609</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" ref="O20:O26" si="80">_xlfn.ACOTH(A20)</f>
+        <v>0.54930614433405489</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" ref="P20:P26" si="81">_xlfn.CSC(A20)</f>
+        <v>1.0997501702946164</v>
+      </c>
+      <c r="Q20" s="2">
+        <f t="shared" ref="Q20:Q26" si="82">_xlfn.CSCH(A20)</f>
+        <v>0.27572056477178319</v>
+      </c>
+      <c r="R20" s="2">
+        <f t="shared" ref="R20:R26" si="83">_xlfn.SECH(A20)</f>
+        <v>0.26580222883407972</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="67"/>
+        <v>0.91294525072762767</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="68"/>
+        <v>0.40808206181339196</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="69"/>
+        <v>2.2371609442247422</v>
+      </c>
+      <c r="E21" s="2" t="e">
+        <f t="shared" si="70"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F21" s="2" t="e">
+        <f t="shared" si="71"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="72"/>
+        <v>1.5208379310729538</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="73"/>
+        <v>242582597.70489514</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="74"/>
+        <v>242582597.70489514</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="75"/>
+        <v>1</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="76"/>
+        <v>3.6895038689889059</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="77"/>
+        <v>3.6882538673612966</v>
+      </c>
+      <c r="M21" s="2" t="e">
+        <f t="shared" si="78"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="79"/>
+        <v>4.9958395721942765E-2</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="80"/>
+        <v>5.0041729278491272E-2</v>
+      </c>
+      <c r="P21" s="2">
+        <f t="shared" si="81"/>
+        <v>1.0953559364080034</v>
+      </c>
+      <c r="Q21" s="2">
+        <f t="shared" si="82"/>
+        <v>4.1223072448771157E-9</v>
+      </c>
+      <c r="R21" s="2">
+        <f t="shared" si="83"/>
+        <v>4.1223072448771157E-9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="67"/>
+        <v>-0.98803162409286183</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="68"/>
+        <v>0.15425144988758405</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="69"/>
+        <v>-6.4053311966462756</v>
+      </c>
+      <c r="E22" s="2" t="e">
+        <f t="shared" si="70"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F22" s="2" t="e">
+        <f t="shared" si="71"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="72"/>
+        <v>1.5374753309166493</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="73"/>
+        <v>5343237290762.2314</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="74"/>
+        <v>5343237290762.2314</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="75"/>
+        <v>1</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="76"/>
+        <v>4.0946222243305304</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="77"/>
+        <v>4.0940666686320855</v>
+      </c>
+      <c r="M22" s="2" t="e">
+        <f t="shared" si="78"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="79"/>
+        <v>3.3320995878247196E-2</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="80"/>
+        <v>3.3345687249336113E-2</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="81"/>
+        <v>-1.012113353070178</v>
+      </c>
+      <c r="Q22" s="2">
+        <f t="shared" si="82"/>
+        <v>1.8715245937680347E-13</v>
+      </c>
+      <c r="R22" s="2">
+        <f t="shared" si="83"/>
+        <v>1.8715245937680347E-13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15">
+      <c r="A23">
+        <v>-2</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="67"/>
+        <v>-0.90929742682568171</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="68"/>
+        <v>-0.41614683654714241</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="69"/>
+        <v>2.1850398632615189</v>
+      </c>
+      <c r="E23" s="2" t="e">
+        <f t="shared" si="70"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F23" s="2" t="e">
+        <f t="shared" si="71"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="72"/>
+        <v>-1.1071487177940904</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="73"/>
+        <v>-3.626860407847019</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="74"/>
+        <v>3.7621956910836314</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="75"/>
+        <v>-0.96402758007581701</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="76"/>
+        <v>-1.4436354751788103</v>
+      </c>
+      <c r="L23" s="2" t="e">
+        <f t="shared" si="77"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M23" s="2" t="e">
+        <f t="shared" si="78"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="79"/>
+        <v>2.677945044588987</v>
+      </c>
+      <c r="O23" s="2">
+        <f t="shared" si="80"/>
+        <v>-0.54930614433405489</v>
+      </c>
+      <c r="P23" s="2">
+        <f t="shared" si="81"/>
+        <v>-1.0997501702946164</v>
+      </c>
+      <c r="Q23" s="2">
+        <f t="shared" si="82"/>
+        <v>-0.27572056477178319</v>
+      </c>
+      <c r="R23" s="2">
+        <f t="shared" si="83"/>
+        <v>0.26580222883407972</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="15">
+      <c r="A24">
+        <v>-7</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="67"/>
+        <v>-0.65698659871878906</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="68"/>
+        <v>0.7539022543433046</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="69"/>
+        <v>-0.87144798272431878</v>
+      </c>
+      <c r="E24" s="2" t="e">
+        <f t="shared" si="70"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F24" s="2" t="e">
+        <f t="shared" si="71"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="72"/>
+        <v>-1.4288992721907328</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="73"/>
+        <v>-548.31612327324649</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="74"/>
+        <v>548.31703515521201</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="75"/>
+        <v>-0.99999833694394469</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="76"/>
+        <v>-2.644120761058629</v>
+      </c>
+      <c r="L24" s="2" t="e">
+        <f t="shared" si="77"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M24" s="2" t="e">
+        <f t="shared" si="78"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="79"/>
+        <v>2.9996955989856291</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="80"/>
+        <v>-0.14384103622589045</v>
+      </c>
+      <c r="P24" s="2">
+        <f t="shared" si="81"/>
+        <v>-1.5221010625637303</v>
+      </c>
+      <c r="Q24" s="2">
+        <f t="shared" si="82"/>
+        <v>-1.823765447622379E-3</v>
+      </c>
+      <c r="R24" s="2">
+        <f t="shared" si="83"/>
+        <v>1.823762414598208E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15">
+      <c r="A25">
+        <v>-100</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="67"/>
+        <v>0.50636564110975879</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="68"/>
+        <v>0.86231887228768389</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="69"/>
+        <v>0.58721391515692911</v>
+      </c>
+      <c r="E25" s="2" t="e">
+        <f t="shared" si="70"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F25" s="2" t="e">
+        <f t="shared" si="71"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="72"/>
+        <v>-1.5607966601082315</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="73"/>
+        <v>-1.3440585709080678E+43</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="74"/>
+        <v>1.3440585709080678E+43</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="75"/>
+        <v>-1</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="76"/>
+        <v>-5.2983423656105888</v>
+      </c>
+      <c r="L25" s="2" t="e">
+        <f t="shared" si="77"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M25" s="2" t="e">
+        <f t="shared" si="78"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="79"/>
+        <v>3.131592986903128</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="80"/>
+        <v>-1.0000333353334763E-2</v>
+      </c>
+      <c r="P25" s="2">
+        <f t="shared" si="81"/>
+        <v>1.9748575314240999</v>
+      </c>
+      <c r="Q25" s="2">
+        <f t="shared" si="82"/>
+        <v>-7.4401519520416712E-44</v>
+      </c>
+      <c r="R25" s="2">
+        <f t="shared" si="83"/>
+        <v>7.4401519520416712E-44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15">
+      <c r="A26">
+        <v>100</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="67"/>
+        <v>-0.50636564110975879</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="68"/>
+        <v>0.86231887228768389</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="69"/>
+        <v>-0.58721391515692911</v>
+      </c>
+      <c r="E26" s="2" t="e">
+        <f t="shared" si="70"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F26" s="2" t="e">
+        <f t="shared" si="71"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="72"/>
+        <v>1.5607966601082315</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="73"/>
+        <v>1.3440585709080678E+43</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="74"/>
+        <v>1.3440585709080678E+43</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="75"/>
+        <v>1</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="76"/>
+        <v>5.2983423656105888</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="77"/>
+        <v>5.298292365610485</v>
+      </c>
+      <c r="M26" s="2" t="e">
+        <f t="shared" si="78"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="79"/>
+        <v>9.9996666866652376E-3</v>
+      </c>
+      <c r="O26" s="2">
+        <f t="shared" si="80"/>
+        <v>1.0000333353334763E-2</v>
+      </c>
+      <c r="P26" s="2">
+        <f t="shared" si="81"/>
+        <v>-1.9748575314240999</v>
+      </c>
+      <c r="Q26" s="2">
+        <f t="shared" si="82"/>
+        <v>7.4401519520416712E-44</v>
+      </c>
+      <c r="R26" s="2">
+        <f t="shared" si="83"/>
+        <v>7.4401519520416712E-44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE7F49B-F42F-4B1D-BCA3-3F938AB4B063}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>9999999999999</v>
+      </c>
+      <c r="B2" s="2">
+        <f>_xlfn.COTH(A2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2">
+        <f t="shared" ref="B3:B7" si="0">_xlfn.COTH(A3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000001872</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>-20</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>-13.2</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000068496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>